<commit_message>
Corrigi problemas em 10/19, 12/19, 05/20
</commit_message>
<xml_diff>
--- a/mpes/src/output_test/2020_05_remu.xlsx
+++ b/mpes/src/output_test/2020_05_remu.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Ministério Público do Estado do Espírito Santo</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t xml:space="preserve">PJ CRIMINAL DE VITÓRIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">OBS: OS VALORES NEGATIVOS REFEREM-SE A DESCONTOS REALIZADOS DENTRO DO MÊS.</t>
@@ -283,15 +286,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -349,9 +352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>956880</xdr:colOff>
+      <xdr:colOff>956520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>195480</xdr:rowOff>
+      <xdr:rowOff>195120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -364,8 +367,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="606960" y="0"/>
-          <a:ext cx="813960" cy="500040"/>
+          <a:off x="606240" y="0"/>
+          <a:ext cx="813600" cy="499680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -385,23 +388,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1048576"/>
+  <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A271" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.33"/>
@@ -594,10 +597,13 @@
       <c r="R7" s="15" t="n">
         <v>27510.15</v>
       </c>
+      <c r="S7" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" s="16" customFormat="true" ht="6.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>

</xml_diff>